<commit_message>
update start and end ulift
</commit_message>
<xml_diff>
--- a/ValidationStartEnd.xlsx
+++ b/ValidationStartEnd.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u0117545\Documents\GitHub\ULIFT_BC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8482627D-8523-4D23-AE3F-8B9DCA9AC6AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62A44306-529C-49AD-B0AC-3BC2D8969230}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6896A571-C2CF-4ED1-96F5-06C70933E9EA}"/>
   </bookViews>
@@ -451,7 +451,7 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -984,7 +984,7 @@
         <v>10</v>
       </c>
       <c r="C29">
-        <v>11</v>
+        <v>70</v>
       </c>
       <c r="D29">
         <v>337</v>

</xml_diff>

<commit_message>
SPM prep added phase 4
</commit_message>
<xml_diff>
--- a/ValidationStartEnd.xlsx
+++ b/ValidationStartEnd.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u0117545\Documents\GitHub\ULIFT_BC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62A44306-529C-49AD-B0AC-3BC2D8969230}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3899E9E-92E5-4012-9D86-832FAC5A60BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6896A571-C2CF-4ED1-96F5-06C70933E9EA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6896A571-C2CF-4ED1-96F5-06C70933E9EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="22">
   <si>
     <t>subj_id</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>BC_003</t>
+  </si>
+  <si>
+    <t>BC_005</t>
   </si>
 </sst>
 </file>
@@ -448,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08C7F914-0B0E-40EC-93CB-7F6B04B8F5B0}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1044,7 +1047,7 @@
         <v>1623</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>20</v>
       </c>
@@ -1064,7 +1067,7 @@
         <v>1609</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -1084,7 +1087,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>20</v>
       </c>
@@ -1092,7 +1095,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>20</v>
       </c>
@@ -1112,7 +1115,7 @@
         <v>1643</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>20</v>
       </c>
@@ -1130,6 +1133,165 @@
       </c>
       <c r="F37">
         <v>1680</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>21</v>
+      </c>
+      <c r="B38" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>21</v>
+      </c>
+      <c r="B39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39">
+        <v>46</v>
+      </c>
+      <c r="D39">
+        <v>355</v>
+      </c>
+      <c r="E39">
+        <v>1104</v>
+      </c>
+      <c r="F39">
+        <v>1402</v>
+      </c>
+      <c r="G39">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>21</v>
+      </c>
+      <c r="B40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40">
+        <v>130</v>
+      </c>
+      <c r="D40">
+        <v>406</v>
+      </c>
+      <c r="E40">
+        <v>1124</v>
+      </c>
+      <c r="F40">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41">
+        <v>49</v>
+      </c>
+      <c r="D41">
+        <v>399</v>
+      </c>
+      <c r="E41">
+        <v>1161</v>
+      </c>
+      <c r="F41">
+        <v>1496</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>21</v>
+      </c>
+      <c r="B42" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42">
+        <v>53</v>
+      </c>
+      <c r="D42">
+        <v>393</v>
+      </c>
+      <c r="E42">
+        <v>1124</v>
+      </c>
+      <c r="F42">
+        <v>1454</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>21</v>
+      </c>
+      <c r="B43" t="s">
+        <v>12</v>
+      </c>
+      <c r="C43">
+        <v>114</v>
+      </c>
+      <c r="D43">
+        <v>425</v>
+      </c>
+      <c r="E43">
+        <v>1137</v>
+      </c>
+      <c r="F43">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>21</v>
+      </c>
+      <c r="B44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>21</v>
+      </c>
+      <c r="B45" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>21</v>
+      </c>
+      <c r="B46" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>21</v>
+      </c>
+      <c r="B47" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>21</v>
+      </c>
+      <c r="B48" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>21</v>
+      </c>
+      <c r="B49" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>